<commit_message>
readme updated + sql samples pret + rectification pts uses
</commit_message>
<xml_diff>
--- a/Points/points détaillés.xlsx
+++ b/Points/points détaillés.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\ing1\s2\dev web\projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ProjetDevWeb\projet_info_2025\Points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F9D5CF-048B-45AE-9E0F-2DF551523066}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5A2546-9D4D-405E-97B6-DDBE8DD66435}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7E314538-0163-4AF4-B2B1-889699F20380}"/>
   </bookViews>
@@ -332,15 +332,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -359,6 +350,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD2542B-8749-421A-8086-7DFA5179D58F}">
   <dimension ref="B1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,564 +696,564 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="J2" s="1" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="J2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
-      <c r="R2" s="18" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
+      <c r="R2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="13" t="s">
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="13" t="s">
+      <c r="M3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="19" t="s">
+      <c r="O3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="15">
+      <c r="S3" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="10" t="s">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="10" t="s">
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="R4" s="20" t="s">
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="14">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="7">
-        <v>1</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="17">
-        <v>1000</v>
-      </c>
-    </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="7">
-        <v>1</v>
-      </c>
-      <c r="L6" s="12" t="s">
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="12" t="s">
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="6">
-        <v>1</v>
-      </c>
-      <c r="L7" s="11" t="s">
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="11" t="s">
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="3"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="9" t="s">
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
-      <c r="J12" s="10" t="s">
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="10" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="5">
-        <v>2</v>
-      </c>
-      <c r="N12" s="10" t="s">
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="12" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="7">
-        <v>2</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="7">
-        <v>2</v>
-      </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="12" t="s">
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="7">
-        <v>2</v>
-      </c>
-      <c r="N13" s="12" t="s">
+      <c r="M13" s="4">
+        <v>2</v>
+      </c>
+      <c r="N13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="12" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="7">
-        <v>2</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="7">
-        <v>2</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="11" t="s">
+      <c r="G14" s="4">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="11" t="s">
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="12" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="11" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="3"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="21"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J18" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="13" t="s">
+      <c r="J18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="13" t="s">
+      <c r="M18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="J19" s="10" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="J19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="10" t="s">
+      <c r="K19" s="2"/>
+      <c r="L19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M19" s="5">
-        <v>1</v>
-      </c>
-      <c r="N19" s="10" t="s">
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="13" t="s">
+      <c r="B20" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="E20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="12" t="s">
+      <c r="G20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="7">
-        <v>1</v>
-      </c>
-      <c r="N20" s="12" t="s">
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="5">
-        <v>1</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="11" t="s">
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="6">
-        <v>2</v>
-      </c>
-      <c r="N21" s="11" t="s">
+      <c r="M21" s="3">
+        <v>2</v>
+      </c>
+      <c r="N21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="12" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="11"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="11" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>